<commit_message>
Add new database entries and update .gitignore
Added a large set of new database entries to databases_processed.json, expanding coverage of resources in genomics, medical, protein, tools, microbiology, and other categories. Updated .gitignore to exclude Python files (*.py).
</commit_message>
<xml_diff>
--- a/nar2025databases.xlsx
+++ b/nar2025databases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="520">
   <si>
     <r>
       <rPr>
@@ -178,16 +178,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BGC Atlas</t>
-    </r>
+    <t>BGC Atlas</t>
   </si>
   <si>
     <t>https://bgc-atlas.cs.uni-tuebingen.de</t>
@@ -2061,6 +2052,900 @@
       </rPr>
       <t>xQTL at cellular resolution</t>
     </r>
+  </si>
+  <si>
+    <t>COVID19db</t>
+  </si>
+  <si>
+    <t>http://www.biomedical-web.com/covid19db</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 transcriptomics and drug discovery</t>
+  </si>
+  <si>
+    <t>Ensembl COVID-19 resource</t>
+  </si>
+  <si>
+    <t>https://covid-19.ensembl.org</t>
+  </si>
+  <si>
+    <t>Integrated public SARS-CoV-2 data</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>http://clingen.igib.res.in/esc</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 immune escape variants</t>
+  </si>
+  <si>
+    <t>SCoV2-MD</t>
+  </si>
+  <si>
+    <t>http://www.scov2-md.org</t>
+  </si>
+  <si>
+    <t>Molecular dynamics of SARS-CoV-2 proteins and variant interpretation</t>
+  </si>
+  <si>
+    <t>SCovid</t>
+  </si>
+  <si>
+    <t>http://bio-annotation.cn/scovid</t>
+  </si>
+  <si>
+    <t>Single cell transcriptomics of SARS-CoV-2 infection</t>
+  </si>
+  <si>
+    <t>T-cell COVID-19 Atlas</t>
+  </si>
+  <si>
+    <t>https://t-cov.hse.ru</t>
+  </si>
+  <si>
+    <t>Predicted affinities between SARS-CoV-2 peptides and HLA alleles</t>
+  </si>
+  <si>
+    <t>VarEPS</t>
+  </si>
+  <si>
+    <t>https://nmdc.cn/ncovn</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 variants, known and theoretical, versus therapies</t>
+  </si>
+  <si>
+    <t>3′aQTL-atlas</t>
+  </si>
+  <si>
+    <t>https://wlcb.oit.uci.edu/3aQTLatlas</t>
+  </si>
+  <si>
+    <t>3′UTR alternative polyadenylation quantitative trait loci</t>
+  </si>
+  <si>
+    <t>AlphaFold Protein Structure Database</t>
+  </si>
+  <si>
+    <t>https://alphafold.ebi.ac.uk</t>
+  </si>
+  <si>
+    <t>Protein structures predicted by AlphaFold</t>
+  </si>
+  <si>
+    <t>Animal-eRNAdb</t>
+  </si>
+  <si>
+    <t>http://gong_lab.hzau.edu.cn/Animal-eRNAdb</t>
+  </si>
+  <si>
+    <t>Animal enhancer RNAs</t>
+  </si>
+  <si>
+    <t>AMDB</t>
+  </si>
+  <si>
+    <t>http://leb.snu.ac.kr/amdb</t>
+  </si>
+  <si>
+    <t>Animal Microbiome Database</t>
+  </si>
+  <si>
+    <t>ASMdb</t>
+  </si>
+  <si>
+    <t>http://www.dna-asmdb.com</t>
+  </si>
+  <si>
+    <t>Allele-Specific DNA Methylation Database</t>
+  </si>
+  <si>
+    <t>ARTS-DB</t>
+  </si>
+  <si>
+    <t>https://arts-db.ziemertlab.com</t>
+  </si>
+  <si>
+    <t>Database for Antibiotic Resistant Targets</t>
+  </si>
+  <si>
+    <t>BrainBase</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/brainbase</t>
+  </si>
+  <si>
+    <t>Brain disease knowledgebase</t>
+  </si>
+  <si>
+    <t>CancerMIRNome</t>
+  </si>
+  <si>
+    <t>http://bioinfo.jialab-ucr.org/CancerMIRNome</t>
+  </si>
+  <si>
+    <t>miRNA profiles in cancer</t>
+  </si>
+  <si>
+    <t>CancerSCEM</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/cancerscem</t>
+  </si>
+  <si>
+    <t>Human cancer single-cell gene expression</t>
+  </si>
+  <si>
+    <t>CeDR</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/cedr</t>
+  </si>
+  <si>
+    <t>Drug responses in health and disease from scRNA-seq</t>
+  </si>
+  <si>
+    <t>CircleBase</t>
+  </si>
+  <si>
+    <t>http://circlebase.maolab.org</t>
+  </si>
+  <si>
+    <t>Human extrachromosomal circular DNA</t>
+  </si>
+  <si>
+    <t>circMine</t>
+  </si>
+  <si>
+    <t>http://www.biomedical-web.com/circmine or http://hpcc.siat.ac.cn/circmine</t>
+  </si>
+  <si>
+    <t>Human circRNA transcriptome in health and disease</t>
+  </si>
+  <si>
+    <t>CompoDynamics</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/compodynamics</t>
+  </si>
+  <si>
+    <t>Sequence composition and characteristics across genomes</t>
+  </si>
+  <si>
+    <t>ConVarT</t>
+  </si>
+  <si>
+    <t>https://convart.org</t>
+  </si>
+  <si>
+    <t>Orthologous variants between human, mouse and worm</t>
+  </si>
+  <si>
+    <t>CovPDB</t>
+  </si>
+  <si>
+    <t>http://www.pharmbioinf.uni-freiburg.de/covpdb</t>
+  </si>
+  <si>
+    <t>Covalent inhibitors and their complexes</t>
+  </si>
+  <si>
+    <t>CTR-DB</t>
+  </si>
+  <si>
+    <t>http://ctrdb.ncpsb.org.cn</t>
+  </si>
+  <si>
+    <t>Patient-derived clinical transcriptomes and drug responses</t>
+  </si>
+  <si>
+    <t>CyanoOmicsDB</t>
+  </si>
+  <si>
+    <t>http://www.cyanoomics.cn</t>
+  </si>
+  <si>
+    <t>Cyanobacteria genomics and transcriptomics</t>
+  </si>
+  <si>
+    <t>DDinter</t>
+  </si>
+  <si>
+    <t>http://ddinter.scbdd.com</t>
+  </si>
+  <si>
+    <t>Drug-drug interactions</t>
+  </si>
+  <si>
+    <t>DISCO</t>
+  </si>
+  <si>
+    <t>https://www.immunesinglecell.org</t>
+  </si>
+  <si>
+    <t>Deep Integration of Single-Cell Omics</t>
+  </si>
+  <si>
+    <t>dNTPpoolDB</t>
+  </si>
+  <si>
+    <t>https://dntppool.org</t>
+  </si>
+  <si>
+    <t>dNTP concentrations in vivo</t>
+  </si>
+  <si>
+    <t>EVA</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/eva</t>
+  </si>
+  <si>
+    <t>European Variation Archive</t>
+  </si>
+  <si>
+    <t>EWAS Open Platform</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/ewas</t>
+  </si>
+  <si>
+    <t>Analysis platform for EWAS research</t>
+  </si>
+  <si>
+    <t>Gene Expression Nebulas</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/gen</t>
+  </si>
+  <si>
+    <t>Expression profiles across species, bulk and single cell</t>
+  </si>
+  <si>
+    <t>GPEdit</t>
+  </si>
+  <si>
+    <t>https://hanlab.uth.edu/GPEdit</t>
+  </si>
+  <si>
+    <t>A-to-I RNA editing in cancer</t>
+  </si>
+  <si>
+    <t>GproteinDb</t>
+  </si>
+  <si>
+    <t>https://gproteindb.org</t>
+  </si>
+  <si>
+    <t>G proteins and their interactions</t>
+  </si>
+  <si>
+    <t>GRAND</t>
+  </si>
+  <si>
+    <t>https://grand.networkmedicine.org</t>
+  </si>
+  <si>
+    <t>Human gene regulation models</t>
+  </si>
+  <si>
+    <t>gutMGene</t>
+  </si>
+  <si>
+    <t>http://bio-annotation.cn/gutmgene</t>
+  </si>
+  <si>
+    <t>Target genes of gut microbes and microbial metabolites in human and mouse</t>
+  </si>
+  <si>
+    <t>huARdb</t>
+  </si>
+  <si>
+    <t>https://huarc.net/database</t>
+  </si>
+  <si>
+    <t>Human Antigen Receptor database</t>
+  </si>
+  <si>
+    <t>Human Proteoform Atlas</t>
+  </si>
+  <si>
+    <t>http://human-proteoform-atlas.org</t>
+  </si>
+  <si>
+    <t>Human proteoforms</t>
+  </si>
+  <si>
+    <t>INDI</t>
+  </si>
+  <si>
+    <t>http://research.naturalantibody.com/nanobodies</t>
+  </si>
+  <si>
+    <t>Integrated Nanobody Database for Immunoinformatics</t>
+  </si>
+  <si>
+    <t>qPTMplants</t>
+  </si>
+  <si>
+    <t>http://qptmplants.omicsbio.info</t>
+  </si>
+  <si>
+    <t>Plant PTMs, including quantitation</t>
+  </si>
+  <si>
+    <t>Kincore</t>
+  </si>
+  <si>
+    <t>http://dunbrack3.fccc.edu/kincore</t>
+  </si>
+  <si>
+    <t>Protein kinase sequence, structure and phylogeny</t>
+  </si>
+  <si>
+    <t>LIRBase</t>
+  </si>
+  <si>
+    <t>https://venyao.xyz/lirbase</t>
+  </si>
+  <si>
+    <t>Long Inverted Repeats in eukaryotes</t>
+  </si>
+  <si>
+    <t>lncRNAfunc</t>
+  </si>
+  <si>
+    <t>https://ccsm.uth.edu/lncRNAfunc</t>
+  </si>
+  <si>
+    <t>Regulatory roles of lncRNAs in cancer</t>
+  </si>
+  <si>
+    <t>m5C-Atlas</t>
+  </si>
+  <si>
+    <t>http://www.xjtlu.edu.cn/biologicalsciences/m5c-atlas</t>
+  </si>
+  <si>
+    <t>The 5-methylcytosine (m5C) epitranscriptome</t>
+  </si>
+  <si>
+    <t>mBodyMap</t>
+  </si>
+  <si>
+    <t>https://mbodymap.microbiome.cloud/#/mbodymap</t>
+  </si>
+  <si>
+    <t>Distribution of microbes across the human body in health and disease</t>
+  </si>
+  <si>
+    <t>MetazExp</t>
+  </si>
+  <si>
+    <t>http://bioinfo.njau.edu.cn/metaExp</t>
+  </si>
+  <si>
+    <t>Analysis of gene expression and alternative splicing in metazoans</t>
+  </si>
+  <si>
+    <t>miTED</t>
+  </si>
+  <si>
+    <t>http://microrna.gr/mited</t>
+  </si>
+  <si>
+    <t>microRNA Tissue Expression Database</t>
+  </si>
+  <si>
+    <t>msRepDB</t>
+  </si>
+  <si>
+    <t>https://msrepdb.cbrc.kaust.edu.sa/pages/msRepDB/index.html</t>
+  </si>
+  <si>
+    <t>multi-species Repeat DataBase</t>
+  </si>
+  <si>
+    <t>MVIP</t>
+  </si>
+  <si>
+    <t>https://mvip.whu.edu.cn</t>
+  </si>
+  <si>
+    <t>Multi-omics Portal of Viral Infection</t>
+  </si>
+  <si>
+    <t>Nanobase.org</t>
+  </si>
+  <si>
+    <t>https://nanobase.org</t>
+  </si>
+  <si>
+    <t>DNA, RNA or protein-DNA/RNA hybrid nanostructures</t>
+  </si>
+  <si>
+    <t>NCATS Inxight: Drugs</t>
+  </si>
+  <si>
+    <t>https://drugs.ncats.io</t>
+  </si>
+  <si>
+    <t>Drugs, their properties and regulation</t>
+  </si>
+  <si>
+    <t>NMDC Data Portal</t>
+  </si>
+  <si>
+    <t>https://data.microbiomedata.org</t>
+  </si>
+  <si>
+    <t>Multi-omics microbiome data</t>
+  </si>
+  <si>
+    <t>NPCDR</t>
+  </si>
+  <si>
+    <t>https://idrblab.org/npcdr or http://npcdr.idrblab.net</t>
+  </si>
+  <si>
+    <t>Drug-Natural Product combinations and diseases</t>
+  </si>
+  <si>
+    <t>NP-MRD</t>
+  </si>
+  <si>
+    <t>http://np-mrd.org</t>
+  </si>
+  <si>
+    <t>Natural Products Magnetic Resonance Database</t>
+  </si>
+  <si>
+    <t>OlfactionBase</t>
+  </si>
+  <si>
+    <t>https://olfab.iiita.ac.in/olfactionbase</t>
+  </si>
+  <si>
+    <t>Odors, Odorants and Olfactory Receptors</t>
+  </si>
+  <si>
+    <t>OncoDB</t>
+  </si>
+  <si>
+    <t>http://www.oncodb.org.</t>
+  </si>
+  <si>
+    <t>Gene Expression and Viral Infection in Cancer</t>
+  </si>
+  <si>
+    <t>ONQUADRO</t>
+  </si>
+  <si>
+    <t>http://onquadro.cs.put.poznan.pl</t>
+  </si>
+  <si>
+    <t>DNA and RNA quadruplexes</t>
+  </si>
+  <si>
+    <t>PCMDB</t>
+  </si>
+  <si>
+    <t>http://www.tobaccodb.org/pcmdb</t>
+  </si>
+  <si>
+    <t>Plant Cell Marker Database</t>
+  </si>
+  <si>
+    <t>PlantGSAD</t>
+  </si>
+  <si>
+    <t>http://systemsbiology.cau.edu.cn/PlantGSEAv2</t>
+  </si>
+  <si>
+    <t>Plant gene set annotations</t>
+  </si>
+  <si>
+    <t>PncsHub</t>
+  </si>
+  <si>
+    <t>https://pncshub.erc.monash.edu</t>
+  </si>
+  <si>
+    <t>Non-classically secreted proteins in Gram-positive bacteria</t>
+  </si>
+  <si>
+    <t>Pol3Base</t>
+  </si>
+  <si>
+    <t>http://rna.sysu.edu.cn/pol3base/index.php</t>
+  </si>
+  <si>
+    <t>PolIII-transcribed ncRNAs</t>
+  </si>
+  <si>
+    <t>proCHiPdb</t>
+  </si>
+  <si>
+    <t>http://prochipdb.org</t>
+  </si>
+  <si>
+    <t>Chromatin immunoprecipitation database for prokaryotic organisms</t>
+  </si>
+  <si>
+    <t>PopHumanVar</t>
+  </si>
+  <si>
+    <t>https://pophumanvar.uab.cat</t>
+  </si>
+  <si>
+    <t>Causal variants of selective sweeps</t>
+  </si>
+  <si>
+    <t>ProNAB</t>
+  </si>
+  <si>
+    <t>https://web.iitm.ac.in/bioinfo2/pronab</t>
+  </si>
+  <si>
+    <t>Protein-Nucleic Acid Binding affinity</t>
+  </si>
+  <si>
+    <t>Regeneration Roadmap</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/regeneration/index</t>
+  </si>
+  <si>
+    <t>Literature and multi-omics data on cell regeneration</t>
+  </si>
+  <si>
+    <t>R-loopBase</t>
+  </si>
+  <si>
+    <t>https://rloopbase.nju.edu.cn</t>
+  </si>
+  <si>
+    <t>R-loops and R-loop regulators</t>
+  </si>
+  <si>
+    <t>RNAPhaSep</t>
+  </si>
+  <si>
+    <t>http://www.rnaphasep.cn</t>
+  </si>
+  <si>
+    <t>RNAs involved in liquid-liquid phase separation</t>
+  </si>
+  <si>
+    <t>RPS</t>
+  </si>
+  <si>
+    <t>http://rps.renlab.org</t>
+  </si>
+  <si>
+    <t>scAPAatlas</t>
+  </si>
+  <si>
+    <t>http://www.bioailab.com:3838/scAPAatlas</t>
+  </si>
+  <si>
+    <t>scRNAseq-based analysis of alternative polyadenylation across cells, tissues and species</t>
+  </si>
+  <si>
+    <t>scAPAdb</t>
+  </si>
+  <si>
+    <t>http://www.bmibig.cn/scAPAdb</t>
+  </si>
+  <si>
+    <t>scEnhancer</t>
+  </si>
+  <si>
+    <t>http://enhanceratlas.net/scenhancer</t>
+  </si>
+  <si>
+    <t>Single-cell enhancer resource</t>
+  </si>
+  <si>
+    <t>scMethBank</t>
+  </si>
+  <si>
+    <t>https://ngdc.cncb.ac.cn/methbank/scm</t>
+  </si>
+  <si>
+    <t>Single Cell methylation data</t>
+  </si>
+  <si>
+    <t>SomaMutDB</t>
+  </si>
+  <si>
+    <t>https://vijglab.einsteinmed.org/SomaMutDB</t>
+  </si>
+  <si>
+    <t>Somatic mutations in normal human tissues</t>
+  </si>
+  <si>
+    <t>SPENCER</t>
+  </si>
+  <si>
+    <t>http://spencer.renlab.org</t>
+  </si>
+  <si>
+    <t>Cancer-associated ncRNA-encoded small peptides</t>
+  </si>
+  <si>
+    <t>SPICA</t>
+  </si>
+  <si>
+    <t>https://spica.unil.ch</t>
+  </si>
+  <si>
+    <t>Swiss Portal for Immune Cell Analysis</t>
+  </si>
+  <si>
+    <t>SYNBIP</t>
+  </si>
+  <si>
+    <t>https://idrblab.org/synbip</t>
+  </si>
+  <si>
+    <t>Synthetic binding proteins</t>
+  </si>
+  <si>
+    <t>TcoFBase</t>
+  </si>
+  <si>
+    <t>http://bio.liclab.net/TcoFbase</t>
+  </si>
+  <si>
+    <t>Transcription cofactors in human and mouse</t>
+  </si>
+  <si>
+    <t>TF-Marker</t>
+  </si>
+  <si>
+    <t>http://bio.liclab.net/TF-Marker</t>
+  </si>
+  <si>
+    <t>Human transcription factors, especially as cell markers</t>
+  </si>
+  <si>
+    <t>TISMO</t>
+  </si>
+  <si>
+    <t>http://tismo.cistrome.org</t>
+  </si>
+  <si>
+    <t>Mouse syngeneic tumor models</t>
+  </si>
+  <si>
+    <t>TissueNexus</t>
+  </si>
+  <si>
+    <t>https://www.diseaselinks.com/TissueNexus</t>
+  </si>
+  <si>
+    <t>Tissue or cell line functional gene networks</t>
+  </si>
+  <si>
+    <t>TransLnc</t>
+  </si>
+  <si>
+    <t>http://bio-bigdata.hrbmu.edu.cn/TransLnc</t>
+  </si>
+  <si>
+    <t>Coding potential of lncRNAs across tissues, including neoantigens</t>
+  </si>
+  <si>
+    <t>tsRFun</t>
+  </si>
+  <si>
+    <t>http://biomed.nscc-gz.cn/DB/tsRFun</t>
+  </si>
+  <si>
+    <t>tsRNA expression and networks</t>
+  </si>
+  <si>
+    <t>VannoPortal</t>
+  </si>
+  <si>
+    <t>http://mulinlab.org/vportal</t>
+  </si>
+  <si>
+    <t>Human genetic variants vs traits and diseases</t>
+  </si>
+  <si>
+    <t>VEuPathDB</t>
+  </si>
+  <si>
+    <t>http://VEuPathDB.org</t>
+  </si>
+  <si>
+    <t>Eukaryotic pathogens, their vectors and hosts</t>
+  </si>
+  <si>
+    <t>ViMIC</t>
+  </si>
+  <si>
+    <t>http://bmtongji.cn/ViMIC/index.php</t>
+  </si>
+  <si>
+    <t>Virus Mutations, Integration sites and Cis-effects</t>
+  </si>
+  <si>
+    <t>ViroidDB</t>
+  </si>
+  <si>
+    <t>https://viroids.org</t>
+  </si>
+  <si>
+    <t>Viroids and viroid-like circular RNA agents</t>
+  </si>
+  <si>
+    <t>VThunter</t>
+  </si>
+  <si>
+    <t>https://db.cngb.org/VThunter</t>
+  </si>
+  <si>
+    <t>scRNA-seq-based analysis of virus receptor expression across animals</t>
+  </si>
+  <si>
+    <t>webTWAS</t>
+  </si>
+  <si>
+    <t>http://www.webtwas.net</t>
+  </si>
+  <si>
+    <t>Transcriptome-Wide Association Studies</t>
+  </si>
+  <si>
+    <t>ZOVER</t>
+  </si>
+  <si>
+    <t>http://www.mgc.ac.cn/cgi-bin/ZOVER/main.cgi</t>
+  </si>
+  <si>
+    <t>Zoonotic and vector-borne viruses</t>
+  </si>
+  <si>
+    <t>BRAD</t>
+  </si>
+  <si>
+    <t>http://brassicadb.cn</t>
+  </si>
+  <si>
+    <t>Brassica Database</t>
+  </si>
+  <si>
+    <t>CPLM</t>
+  </si>
+  <si>
+    <t>http://cplm.biocuckoo.cn</t>
+  </si>
+  <si>
+    <t>Compendium of Protein Lysine Modifications</t>
+  </si>
+  <si>
+    <t>DRAMP</t>
+  </si>
+  <si>
+    <t>http://dramp.cpu-bioinfor.org</t>
+  </si>
+  <si>
+    <t>Antimicrobial peptides</t>
+  </si>
+  <si>
+    <t>Echinobase</t>
+  </si>
+  <si>
+    <t>https://www.echinobase.org</t>
+  </si>
+  <si>
+    <t>Echinoderm genomics</t>
+  </si>
+  <si>
+    <t>EGA</t>
+  </si>
+  <si>
+    <t>https://ega-archive.org</t>
+  </si>
+  <si>
+    <t>European Genome-Phenome Archive</t>
+  </si>
+  <si>
+    <t>GTDB</t>
+  </si>
+  <si>
+    <t>http://gtdb.ecogenomic.org</t>
+  </si>
+  <si>
+    <t>Genome Taxonomy Database</t>
+  </si>
+  <si>
+    <t>LPSN and TYGS</t>
+  </si>
+  <si>
+    <t>https://lpsn.dsmz.de, https://tygs.dsmz.de</t>
+  </si>
+  <si>
+    <t>List of Prokaryotic names with Standing in Nomenclature and Type (Strain) Genome Server</t>
+  </si>
+  <si>
+    <t>NPAtlas</t>
+  </si>
+  <si>
+    <t>https://www.npatlas.org</t>
+  </si>
+  <si>
+    <t>Natural Products Atlas</t>
+  </si>
+  <si>
+    <t>OncoSplicing</t>
+  </si>
+  <si>
+    <t>http://www.oncosplicing.com</t>
+  </si>
+  <si>
+    <t>Alternative splicing and cancer</t>
+  </si>
+  <si>
+    <t>Priority index</t>
+  </si>
+  <si>
+    <t>http://pi.well.ox.ac.uk</t>
+  </si>
+  <si>
+    <t>Drug targets for immune-mediated diseases</t>
+  </si>
+  <si>
+    <t>RGD</t>
+  </si>
+  <si>
+    <t>http://animal.nwsuaf.edu.cn/RGD</t>
+  </si>
+  <si>
+    <t>Ruminant Genome Database</t>
+  </si>
+  <si>
+    <t>SignaLink</t>
+  </si>
+  <si>
+    <t>https://slk3.netbiol.org</t>
+  </si>
+  <si>
+    <t>Tissue-specific signaling networks in model organisms</t>
+  </si>
+  <si>
+    <t>Ubibrowser</t>
+  </si>
+  <si>
+    <t>http://ubibrowser.ncpsb.org.cn/v2</t>
+  </si>
+  <si>
+    <t>Proteome-wide ubiquitin ligase/deubiquitinase-substrate interactions in eukaryotes</t>
   </si>
 </sst>
 </file>
@@ -2700,7 +3585,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2710,8 +3595,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3024,16 +3915,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:A$1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162:C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="49.25" customWidth="1"/>
     <col min="3" max="3" width="79.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3092,7 +3983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" ht="94.5" spans="1:3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -3103,7 +3994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" ht="108" spans="1:3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -3114,8 +4005,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" ht="81" spans="1:3">
-      <c r="A8" s="2" t="s">
+    <row r="8" ht="15" spans="1:3">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3125,7 +4016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" ht="67.5" spans="1:3">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -3136,7 +4027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" ht="67.5" spans="1:3">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -3147,7 +4038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" ht="54" spans="1:3">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -3158,7 +4049,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="54" spans="1:3">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -3169,7 +4060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" ht="40.5" spans="1:3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -3180,7 +4071,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" ht="67.5" spans="1:3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -3191,7 +4082,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" ht="108" spans="1:3">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -3202,7 +4093,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" ht="54" spans="1:3">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
@@ -3213,7 +4104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" ht="108" spans="1:3">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -3224,7 +4115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" ht="40.5" spans="1:3">
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -3235,7 +4126,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" ht="94.5" spans="1:3">
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -3246,7 +4137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" ht="54" spans="1:3">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
@@ -3257,7 +4148,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" ht="175.5" spans="1:3">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -3268,7 +4159,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" ht="40.5" spans="1:3">
+    <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -3279,7 +4170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" ht="54" spans="1:3">
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
@@ -3290,7 +4181,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" ht="54" spans="1:3">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
@@ -3301,7 +4192,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" ht="81" spans="1:3">
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>72</v>
       </c>
@@ -3312,7 +4203,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" ht="81" spans="1:3">
+    <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
@@ -3323,7 +4214,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" ht="67.5" spans="1:3">
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>78</v>
       </c>
@@ -3334,7 +4225,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" ht="121.5" spans="1:3">
+    <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
@@ -3345,7 +4236,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" ht="94.5" spans="1:3">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
@@ -3356,7 +4247,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" ht="94.5" spans="1:3">
+    <row r="30" ht="27" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>87</v>
       </c>
@@ -3367,7 +4258,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" ht="67.5" spans="1:3">
+    <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
@@ -3378,7 +4269,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" ht="94.5" spans="1:3">
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
@@ -3389,7 +4280,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" ht="67.5" spans="1:3">
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
@@ -3400,7 +4291,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" ht="81" spans="1:3">
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>99</v>
       </c>
@@ -3411,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" ht="94.5" spans="1:3">
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>102</v>
       </c>
@@ -3422,7 +4313,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" ht="135" spans="1:3">
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>105</v>
       </c>
@@ -3433,7 +4324,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" ht="81" spans="1:3">
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
         <v>108</v>
       </c>
@@ -3444,7 +4335,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" ht="94.5" spans="1:3">
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
         <v>111</v>
       </c>
@@ -3455,7 +4346,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" ht="54" spans="1:3">
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
         <v>114</v>
       </c>
@@ -3466,7 +4357,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" ht="54" spans="1:3">
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -3477,7 +4368,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" ht="67.5" spans="1:3">
+    <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -3488,7 +4379,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" ht="67.5" spans="1:3">
+    <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
         <v>123</v>
       </c>
@@ -3499,7 +4390,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" ht="108" spans="1:3">
+    <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
         <v>126</v>
       </c>
@@ -3510,7 +4401,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" ht="108" spans="1:3">
+    <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
         <v>129</v>
       </c>
@@ -3521,7 +4412,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" ht="40.5" spans="1:3">
+    <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
         <v>132</v>
       </c>
@@ -3532,7 +4423,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" ht="67.5" spans="1:3">
+    <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
@@ -3543,7 +4434,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" ht="67.5" spans="1:3">
+    <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
@@ -3554,7 +4445,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" ht="108" spans="1:3">
+    <row r="48" ht="27" spans="1:3">
       <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
@@ -3565,7 +4456,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" ht="81" spans="1:3">
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>144</v>
       </c>
@@ -3576,7 +4467,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" ht="67.5" spans="1:3">
+    <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -3587,7 +4478,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" ht="67.5" spans="1:3">
+    <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
         <v>150</v>
       </c>
@@ -3598,7 +4489,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" ht="121.5" spans="1:3">
+    <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
         <v>153</v>
       </c>
@@ -3609,7 +4500,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" ht="94.5" spans="1:3">
+    <row r="53" ht="27" spans="1:3">
       <c r="A53" s="2" t="s">
         <v>156</v>
       </c>
@@ -3620,7 +4511,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" ht="108" spans="1:3">
+    <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
         <v>159</v>
       </c>
@@ -3631,7 +4522,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" ht="94.5" spans="1:3">
+    <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
         <v>162</v>
       </c>
@@ -3642,7 +4533,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" ht="81" spans="1:3">
+    <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
         <v>165</v>
       </c>
@@ -3653,7 +4544,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" ht="121.5" spans="1:3">
+    <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
         <v>168</v>
       </c>
@@ -3664,7 +4555,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="58" ht="81" spans="1:3">
+    <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
         <v>171</v>
       </c>
@@ -3675,7 +4566,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" ht="67.5" spans="1:3">
+    <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
         <v>174</v>
       </c>
@@ -3686,7 +4577,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" ht="67.5" spans="1:3">
+    <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
         <v>177</v>
       </c>
@@ -3697,7 +4588,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="61" ht="108" spans="1:3">
+    <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
         <v>180</v>
       </c>
@@ -3708,18 +4599,18 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" ht="108" spans="1:3">
+    <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="63" ht="81" spans="1:3">
+    <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
         <v>186</v>
       </c>
@@ -3730,7 +4621,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" ht="108" spans="1:3">
+    <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
         <v>189</v>
       </c>
@@ -3741,7 +4632,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" ht="81" spans="1:3">
+    <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
         <v>192</v>
       </c>
@@ -3752,7 +4643,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" ht="67.5" spans="1:3">
+    <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
         <v>195</v>
       </c>
@@ -3763,7 +4654,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="67" ht="121.5" spans="1:3">
+    <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
         <v>198</v>
       </c>
@@ -3774,7 +4665,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" ht="67.5" spans="1:3">
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>201</v>
       </c>
@@ -3785,7 +4676,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" ht="94.5" spans="1:3">
+    <row r="69" ht="27" spans="1:3">
       <c r="A69" s="2" t="s">
         <v>204</v>
       </c>
@@ -3796,7 +4687,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="70" ht="94.5" spans="1:3">
+    <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
         <v>207</v>
       </c>
@@ -3807,7 +4698,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" ht="81" spans="1:3">
+    <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
         <v>210</v>
       </c>
@@ -3818,7 +4709,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" ht="108" spans="1:3">
+    <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
         <v>213</v>
       </c>
@@ -3829,7 +4720,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" ht="81" spans="1:3">
+    <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
         <v>216</v>
       </c>
@@ -3840,7 +4731,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="74" ht="54" spans="1:3">
+    <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
         <v>219</v>
       </c>
@@ -3849,6 +4740,1106 @@
       </c>
       <c r="C74" s="2" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>222</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C75" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" t="s">
+        <v>226</v>
+      </c>
+      <c r="C76" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>231</v>
+      </c>
+      <c r="B78" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>234</v>
+      </c>
+      <c r="B79" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" t="s">
+        <v>238</v>
+      </c>
+      <c r="C80" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" t="s">
+        <v>241</v>
+      </c>
+      <c r="C81" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>243</v>
+      </c>
+      <c r="B82" t="s">
+        <v>244</v>
+      </c>
+      <c r="C82" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>246</v>
+      </c>
+      <c r="B83" t="s">
+        <v>247</v>
+      </c>
+      <c r="C83" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>252</v>
+      </c>
+      <c r="B85" t="s">
+        <v>253</v>
+      </c>
+      <c r="C85" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>255</v>
+      </c>
+      <c r="B86" t="s">
+        <v>256</v>
+      </c>
+      <c r="C86" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>258</v>
+      </c>
+      <c r="B87" t="s">
+        <v>259</v>
+      </c>
+      <c r="C87" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>261</v>
+      </c>
+      <c r="B88" t="s">
+        <v>262</v>
+      </c>
+      <c r="C88" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>264</v>
+      </c>
+      <c r="B89" t="s">
+        <v>265</v>
+      </c>
+      <c r="C89" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>267</v>
+      </c>
+      <c r="B90" t="s">
+        <v>268</v>
+      </c>
+      <c r="C90" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>270</v>
+      </c>
+      <c r="B91" t="s">
+        <v>271</v>
+      </c>
+      <c r="C91" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>273</v>
+      </c>
+      <c r="B92" t="s">
+        <v>274</v>
+      </c>
+      <c r="C92" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>276</v>
+      </c>
+      <c r="B93" t="s">
+        <v>277</v>
+      </c>
+      <c r="C93" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>279</v>
+      </c>
+      <c r="B94" t="s">
+        <v>280</v>
+      </c>
+      <c r="C94" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>282</v>
+      </c>
+      <c r="B95" t="s">
+        <v>283</v>
+      </c>
+      <c r="C95" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>285</v>
+      </c>
+      <c r="B96" t="s">
+        <v>286</v>
+      </c>
+      <c r="C96" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>288</v>
+      </c>
+      <c r="B97" t="s">
+        <v>289</v>
+      </c>
+      <c r="C97" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>291</v>
+      </c>
+      <c r="B98" t="s">
+        <v>292</v>
+      </c>
+      <c r="C98" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>294</v>
+      </c>
+      <c r="B99" t="s">
+        <v>295</v>
+      </c>
+      <c r="C99" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>297</v>
+      </c>
+      <c r="B100" t="s">
+        <v>298</v>
+      </c>
+      <c r="C100" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>300</v>
+      </c>
+      <c r="B101" t="s">
+        <v>301</v>
+      </c>
+      <c r="C101" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>303</v>
+      </c>
+      <c r="B102" t="s">
+        <v>304</v>
+      </c>
+      <c r="C102" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>306</v>
+      </c>
+      <c r="B103" t="s">
+        <v>307</v>
+      </c>
+      <c r="C103" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" t="s">
+        <v>310</v>
+      </c>
+      <c r="C104" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>312</v>
+      </c>
+      <c r="B105" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" t="s">
+        <v>316</v>
+      </c>
+      <c r="C106" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>318</v>
+      </c>
+      <c r="B107" t="s">
+        <v>319</v>
+      </c>
+      <c r="C107" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>321</v>
+      </c>
+      <c r="B108" t="s">
+        <v>322</v>
+      </c>
+      <c r="C108" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>324</v>
+      </c>
+      <c r="B109" t="s">
+        <v>325</v>
+      </c>
+      <c r="C109" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>327</v>
+      </c>
+      <c r="B110" t="s">
+        <v>328</v>
+      </c>
+      <c r="C110" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>330</v>
+      </c>
+      <c r="B111" t="s">
+        <v>331</v>
+      </c>
+      <c r="C111" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>333</v>
+      </c>
+      <c r="B112" t="s">
+        <v>334</v>
+      </c>
+      <c r="C112" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>336</v>
+      </c>
+      <c r="B113" t="s">
+        <v>337</v>
+      </c>
+      <c r="C113" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>339</v>
+      </c>
+      <c r="B114" t="s">
+        <v>340</v>
+      </c>
+      <c r="C114" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>342</v>
+      </c>
+      <c r="B115" t="s">
+        <v>343</v>
+      </c>
+      <c r="C115" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>345</v>
+      </c>
+      <c r="B116" t="s">
+        <v>346</v>
+      </c>
+      <c r="C116" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>348</v>
+      </c>
+      <c r="B117" t="s">
+        <v>349</v>
+      </c>
+      <c r="C117" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>351</v>
+      </c>
+      <c r="B118" t="s">
+        <v>352</v>
+      </c>
+      <c r="C118" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>354</v>
+      </c>
+      <c r="B119" t="s">
+        <v>355</v>
+      </c>
+      <c r="C119" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>357</v>
+      </c>
+      <c r="B120" t="s">
+        <v>358</v>
+      </c>
+      <c r="C120" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>360</v>
+      </c>
+      <c r="B121" t="s">
+        <v>361</v>
+      </c>
+      <c r="C121" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>363</v>
+      </c>
+      <c r="B122" t="s">
+        <v>364</v>
+      </c>
+      <c r="C122" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>366</v>
+      </c>
+      <c r="B123" t="s">
+        <v>367</v>
+      </c>
+      <c r="C123" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>369</v>
+      </c>
+      <c r="B124" t="s">
+        <v>370</v>
+      </c>
+      <c r="C124" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>372</v>
+      </c>
+      <c r="B125" t="s">
+        <v>373</v>
+      </c>
+      <c r="C125" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>375</v>
+      </c>
+      <c r="B126" t="s">
+        <v>376</v>
+      </c>
+      <c r="C126" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>378</v>
+      </c>
+      <c r="B127" t="s">
+        <v>379</v>
+      </c>
+      <c r="C127" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>381</v>
+      </c>
+      <c r="B128" t="s">
+        <v>382</v>
+      </c>
+      <c r="C128" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>384</v>
+      </c>
+      <c r="B129" t="s">
+        <v>385</v>
+      </c>
+      <c r="C129" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>387</v>
+      </c>
+      <c r="B130" t="s">
+        <v>388</v>
+      </c>
+      <c r="C130" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>390</v>
+      </c>
+      <c r="B131" t="s">
+        <v>391</v>
+      </c>
+      <c r="C131" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>393</v>
+      </c>
+      <c r="B132" t="s">
+        <v>394</v>
+      </c>
+      <c r="C132" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>396</v>
+      </c>
+      <c r="B133" t="s">
+        <v>397</v>
+      </c>
+      <c r="C133" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>399</v>
+      </c>
+      <c r="B134" t="s">
+        <v>400</v>
+      </c>
+      <c r="C134" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>402</v>
+      </c>
+      <c r="B135" t="s">
+        <v>403</v>
+      </c>
+      <c r="C135" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>405</v>
+      </c>
+      <c r="B136" t="s">
+        <v>406</v>
+      </c>
+      <c r="C136" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>408</v>
+      </c>
+      <c r="B137" t="s">
+        <v>409</v>
+      </c>
+      <c r="C137" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>411</v>
+      </c>
+      <c r="B138" t="s">
+        <v>412</v>
+      </c>
+      <c r="C138" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>414</v>
+      </c>
+      <c r="B139" t="s">
+        <v>415</v>
+      </c>
+      <c r="C139" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>417</v>
+      </c>
+      <c r="B140" t="s">
+        <v>418</v>
+      </c>
+      <c r="C140" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>419</v>
+      </c>
+      <c r="B141" t="s">
+        <v>420</v>
+      </c>
+      <c r="C141" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>422</v>
+      </c>
+      <c r="B142" t="s">
+        <v>423</v>
+      </c>
+      <c r="C142" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>424</v>
+      </c>
+      <c r="B143" t="s">
+        <v>425</v>
+      </c>
+      <c r="C143" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>427</v>
+      </c>
+      <c r="B144" t="s">
+        <v>428</v>
+      </c>
+      <c r="C144" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>430</v>
+      </c>
+      <c r="B145" t="s">
+        <v>431</v>
+      </c>
+      <c r="C145" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>433</v>
+      </c>
+      <c r="B146" t="s">
+        <v>434</v>
+      </c>
+      <c r="C146" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>436</v>
+      </c>
+      <c r="B147" t="s">
+        <v>437</v>
+      </c>
+      <c r="C147" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>439</v>
+      </c>
+      <c r="B148" t="s">
+        <v>440</v>
+      </c>
+      <c r="C148" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>442</v>
+      </c>
+      <c r="B149" t="s">
+        <v>443</v>
+      </c>
+      <c r="C149" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>445</v>
+      </c>
+      <c r="B150" t="s">
+        <v>446</v>
+      </c>
+      <c r="C150" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>448</v>
+      </c>
+      <c r="B151" t="s">
+        <v>449</v>
+      </c>
+      <c r="C151" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>451</v>
+      </c>
+      <c r="B152" t="s">
+        <v>452</v>
+      </c>
+      <c r="C152" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>454</v>
+      </c>
+      <c r="B153" t="s">
+        <v>455</v>
+      </c>
+      <c r="C153" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>457</v>
+      </c>
+      <c r="B154" t="s">
+        <v>458</v>
+      </c>
+      <c r="C154" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>460</v>
+      </c>
+      <c r="B155" t="s">
+        <v>461</v>
+      </c>
+      <c r="C155" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>463</v>
+      </c>
+      <c r="B156" t="s">
+        <v>464</v>
+      </c>
+      <c r="C156" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>466</v>
+      </c>
+      <c r="B157" t="s">
+        <v>467</v>
+      </c>
+      <c r="C157" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>469</v>
+      </c>
+      <c r="B158" t="s">
+        <v>470</v>
+      </c>
+      <c r="C158" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>472</v>
+      </c>
+      <c r="B159" t="s">
+        <v>473</v>
+      </c>
+      <c r="C159" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>475</v>
+      </c>
+      <c r="B160" t="s">
+        <v>476</v>
+      </c>
+      <c r="C160" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>478</v>
+      </c>
+      <c r="B161" t="s">
+        <v>479</v>
+      </c>
+      <c r="C161" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>481</v>
+      </c>
+      <c r="B162" t="s">
+        <v>482</v>
+      </c>
+      <c r="C162" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>484</v>
+      </c>
+      <c r="B163" t="s">
+        <v>485</v>
+      </c>
+      <c r="C163" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>487</v>
+      </c>
+      <c r="B164" t="s">
+        <v>488</v>
+      </c>
+      <c r="C164" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>490</v>
+      </c>
+      <c r="B165" t="s">
+        <v>491</v>
+      </c>
+      <c r="C165" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>493</v>
+      </c>
+      <c r="B166" t="s">
+        <v>494</v>
+      </c>
+      <c r="C166" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>496</v>
+      </c>
+      <c r="B167" t="s">
+        <v>497</v>
+      </c>
+      <c r="C167" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>499</v>
+      </c>
+      <c r="B168" t="s">
+        <v>500</v>
+      </c>
+      <c r="C168" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>502</v>
+      </c>
+      <c r="B169" t="s">
+        <v>503</v>
+      </c>
+      <c r="C169" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>505</v>
+      </c>
+      <c r="B170" t="s">
+        <v>506</v>
+      </c>
+      <c r="C170" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>508</v>
+      </c>
+      <c r="B171" t="s">
+        <v>509</v>
+      </c>
+      <c r="C171" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>511</v>
+      </c>
+      <c r="B172" t="s">
+        <v>512</v>
+      </c>
+      <c r="C172" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>514</v>
+      </c>
+      <c r="B173" t="s">
+        <v>515</v>
+      </c>
+      <c r="C173" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>517</v>
+      </c>
+      <c r="B174" t="s">
+        <v>518</v>
+      </c>
+      <c r="C174" t="s">
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -3926,6 +5917,7 @@
     <hyperlink ref="B72" r:id="rId71" display="https://transcriptdb.cobius.usherbrooke.ca" tooltip="https://transcriptdb.cobius.usherbrooke.ca"/>
     <hyperlink ref="B73" r:id="rId72" display="https://ngdc.cncb.ac.cn/vdge" tooltip="https://ngdc.cncb.ac.cn/vdge"/>
     <hyperlink ref="B74" r:id="rId73" display="http://www.hitxqtl.org.cn/" tooltip="http://www.hitxqtl.org.cn/"/>
+    <hyperlink ref="B75" r:id="rId74" display="http://www.biomedical-web.com/covid19db"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>